<commit_message>
Amazon e Meli funcionando perfeitamente
</commit_message>
<xml_diff>
--- a/precos/precos_report.xlsx
+++ b/precos/precos_report.xlsx
@@ -481,19 +481,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Gillette Carga Para Aparelho De Barbear Mach3 2 Unidades</t>
-        </is>
-      </c>
-      <c r="C2">
-        <f>HYPERLINK("https://www.amazon.com.br/dp/B00RVUIRN4", "18.01")</f>
+          <t>Carga para Aparelho de Barbear Gillette Mach3 com 2 unidades</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2">
+        <f>HYPERLINK("https://www.mercadolivre.com.br/carga-para-lmina-de-barbear-gillette-mach3-2-unidades/p/MLB17355357", "11.71")</f>
         <v/>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
-        <v>18.01</v>
+        <v>11.71</v>
       </c>
     </row>
     <row r="3">
@@ -502,19 +502,19 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Gillette Carga Para Aparelho De Barbear Fusion5 4 Unidades</t>
-        </is>
-      </c>
-      <c r="C3">
-        <f>HYPERLINK("https://www.amazon.com.br/dp/B07Y36PSZW", "76.98")</f>
+          <t>Carga para Aparelho de Barbear Gillette Fusion 5 - 4 unidades</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3">
+        <f>HYPERLINK("https://www.mercadolivre.com.br/4-cartuchos-refil-para-aparelho-fusion-5-gillette/p/MLB16088319", "87.02")</f>
         <v/>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
-        <v>76.98</v>
+        <v>87.02</v>
       </c>
     </row>
     <row r="4">
@@ -523,19 +523,19 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Gillette Mach3 Carbono Aparelho de barbear reutilizável com Carvão Ativado e Fita Lubrificante Melhorada 1 Ud</t>
-        </is>
-      </c>
-      <c r="C4">
-        <f>HYPERLINK("https://www.amazon.com.br/dp/B0BZCJBV8J", "25.19")</f>
+          <t>Aparelho de Barbear Gillette Mach3 com 1 Unidade</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4">
+        <f>HYPERLINK("https://www.mercadolivre.com.br/aparelho-de-barbear-mach3-carbono-reutilizavel/p/MLB23207098", "26.59")</f>
         <v/>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
-        <v>25.19</v>
+        <v>26.59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>